<commit_message>
added in final example
</commit_message>
<xml_diff>
--- a/untidy_data.xlsx
+++ b/untidy_data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\TidyData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="13605" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="27792" windowHeight="13608" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="merged_cells" sheetId="1" r:id="rId1"/>
@@ -15,13 +20,15 @@
     <sheet name="inconsistent_data" sheetId="6" r:id="rId6"/>
     <sheet name="missing_values" sheetId="7" r:id="rId7"/>
     <sheet name="not_comp_readable" sheetId="8" r:id="rId8"/>
+    <sheet name="undocumented" sheetId="10" r:id="rId9"/>
+    <sheet name="ESRI_MAPINFO_SHEET" sheetId="9" state="veryHidden" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>region</t>
   </si>
@@ -142,8 +149,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="171" formatCode="mm/dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="mm/dd"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -197,17 +204,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -216,6 +220,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -232,8 +239,105 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>294147</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>5045</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="EsriDoNotEdit"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6390147" cy="1650965"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="5000" b="1" i="0" cap="none" spc="0">
+              <a:ln w="18000">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="140000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:noFill/>
+              <a:effectLst>
+                <a:outerShdw blurRad="25500" dist="23000" dir="7020000" algn="tl">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>DO NOT EDIT </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="5000" b="1" i="0" cap="none" spc="0">
+              <a:ln w="18000">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="140000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:noFill/>
+              <a:effectLst>
+                <a:outerShdw blurRad="25500" dist="23000" dir="7020000" algn="tl">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> For Esri use only</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -529,15 +633,15 @@
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -548,7 +652,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -559,7 +663,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -575,6 +679,19 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -586,12 +703,12 @@
       <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -599,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -607,7 +724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -615,7 +732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -636,13 +753,13 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -650,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -658,7 +775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -666,7 +783,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -674,7 +791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -682,7 +799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -690,7 +807,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -698,7 +815,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -706,7 +823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -714,7 +831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -735,12 +852,12 @@
       <selection activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -751,25 +868,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>2500</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>4000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>7000</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>4100</v>
       </c>
     </row>
@@ -786,9 +903,9 @@
       <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -799,22 +916,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>2500</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>9000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>7000</v>
       </c>
       <c r="C3">
@@ -834,14 +951,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -855,7 +972,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -865,15 +982,15 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>25000000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>42729</v>
       </c>
       <c r="C3" t="s">
@@ -883,11 +1000,11 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C4" t="s">
@@ -897,11 +1014,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C5" t="s">
@@ -928,9 +1045,9 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -941,7 +1058,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -952,7 +1069,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -963,7 +1080,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -971,11 +1088,11 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>35</v>
       </c>
     </row>
@@ -988,43 +1105,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>25000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2">
+        <v>15000000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>